<commit_message>
DB-product / project_account/ project_content 추가 , project db 수정 / 마이페이지  수정
</commit_message>
<xml_diff>
--- a/finalp/src/main/webapp/resources/db/MEMBER.xlsx
+++ b/finalp/src/main/webapp/resources/db/MEMBER.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>MEMBER_ID</t>
   </si>
@@ -91,6 +91,22 @@
   </si>
   <si>
     <t>ADDRESS_NUM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test@cornsalad.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -149,7 +165,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -160,6 +176,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -582,11 +601,32 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>